<commit_message>
Updated the Customer Input, Login Page
</commit_message>
<xml_diff>
--- a/Pixel2Program V2.0/Program to Pixel V2.0.xlsx
+++ b/Pixel2Program V2.0/Program to Pixel V2.0.xlsx
@@ -5,21 +5,32 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\U439310\OneDrive - Danfoss\Shared Folders\Danfoss\ALADIN\Pixel2Program V2.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://danfoss-my.sharepoint.com/personal/asish_george_danfoss_com/Documents/Shared Folders/Danfoss/ALADIN/Pixel2Program V2.0/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{060B4B3D-5408-4896-88AC-8DD8C41FA254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
     <sheet name="Database Structure" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -289,7 +300,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -307,7 +318,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -590,8 +600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -778,13 +788,13 @@
       <c r="D23" s="5"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="11" t="s">
+      <c r="A24" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="5" t="s">
         <v>56</v>
       </c>
       <c r="D24" s="5"/>
@@ -806,7 +816,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F055D1F-FB99-4810-A628-B96C17A76ABF}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>